<commit_message>
update pwl pos dari jobsheet 8
</commit_message>
<xml_diff>
--- a/PWLPOS.v2/public/template_data/penjualan.xlsx
+++ b/PWLPOS.v2/public/template_data/penjualan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\Tugas-WebLanjut\PWLPOS.v2\public\template_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{509D3B71-774A-41D8-AD85-CDFB9CD3C977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD295DD-23F8-44A2-BD8F-10DEE30B66F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{75C41F1E-5AF5-4043-8B20-BD82A7E7F480}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>user_id</t>
   </si>
@@ -58,9 +58,6 @@
   </si>
   <si>
     <t>Administrator</t>
-  </si>
-  <si>
-    <t>2025-04-07 12:20:05</t>
   </si>
   <si>
     <t>barang_id</t>
@@ -452,7 +449,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -477,13 +474,13 @@
         <v>0</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -536,8 +533,8 @@
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
-        <v>8</v>
+      <c r="B4" s="1">
+        <v>45754.51394675926</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>

</xml_diff>